<commit_message>
starting on data summary
</commit_message>
<xml_diff>
--- a/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 09_15_2019.xlsx
+++ b/0 - Field Data Sheets/Weir Calibration Field Form 2019 CURRENT 09_15_2019.xlsx
@@ -17,7 +17,7 @@
     <sheet name="ESRI_MAPINFO_SHEET" sheetId="3" state="veryHidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$P$673</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$AA$673</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -2256,7 +2256,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2605,8 +2605,8 @@
   <dimension ref="A1:AA673"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D469" sqref="D469"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H497" sqref="H497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3119,7 +3119,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>43591.527513136578</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>43592.637291597217</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>43594.624838090276</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7">
         <v>43595.711790578702</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="7">
         <v>43598.531430370371</v>
       </c>
@@ -7896,7 +7896,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="148" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="7">
         <v>43599.485035810183</v>
       </c>
@@ -10195,7 +10195,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="219" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A219" s="7">
         <v>43620.531383842594</v>
       </c>
@@ -10247,7 +10247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="7">
         <v>43620.53862825231</v>
       </c>
@@ -10346,7 +10346,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="224" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A224" s="7">
         <v>43620.562107916667</v>
       </c>
@@ -10921,7 +10921,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="243" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="7">
         <v>43633.539491469906</v>
       </c>
@@ -11195,7 +11195,7 @@
         <v>7400</v>
       </c>
     </row>
-    <row r="252" spans="1:15" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A252" s="7">
         <v>43633.63865868056</v>
       </c>
@@ -11218,7 +11218,7 @@
         <v>367</v>
       </c>
       <c r="H252" s="5">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="J252" s="5">
         <v>3.2</v>
@@ -13525,7 +13525,7 @@
       </c>
       <c r="Q321" s="5"/>
     </row>
-    <row r="322" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:17" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="7">
         <v>43647.54435773148</v>
       </c>
@@ -14729,7 +14729,7 @@
         <v>5707</v>
       </c>
     </row>
-    <row r="359" spans="1:16" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="25">
         <v>43661.465437303239</v>
       </c>
@@ -15229,7 +15229,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="375" spans="1:16" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A375" s="25">
         <v>43662.423942743058</v>
       </c>
@@ -15540,7 +15540,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="385" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A385" s="25">
         <v>43662.524749976852</v>
       </c>
@@ -15572,7 +15572,7 @@
         <v>2651</v>
       </c>
     </row>
-    <row r="386" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="25">
         <v>43662.526702222225</v>
       </c>
@@ -15604,7 +15604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A387" s="25">
         <v>43662.528149259262</v>
       </c>
@@ -15632,7 +15632,7 @@
       </c>
       <c r="P387" s="26"/>
     </row>
-    <row r="388" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A388" s="25">
         <v>43662.530195763888</v>
       </c>
@@ -15664,7 +15664,7 @@
         <v>2690</v>
       </c>
     </row>
-    <row r="389" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A389" s="25">
         <v>43662.533871203705</v>
       </c>
@@ -15696,7 +15696,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="390" spans="1:16" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A390" s="25">
         <v>43662.534038217593</v>
       </c>
@@ -15728,7 +15728,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="391" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A391" s="25">
         <v>43662.552655601852</v>
       </c>
@@ -15760,7 +15760,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="392" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A392" s="25">
         <v>43662.553831041667</v>
       </c>
@@ -15792,7 +15792,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="393" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A393" s="25">
         <v>43662.553892222219</v>
       </c>
@@ -15821,7 +15821,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="394" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A394" s="25">
         <v>43662.576265393523</v>
       </c>
@@ -15850,7 +15850,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="395" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A395" s="25">
         <v>43662.605140277781</v>
       </c>
@@ -15882,7 +15882,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="396" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A396" s="25">
         <v>43662.608947546294</v>
       </c>
@@ -15911,7 +15911,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="397" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A397" s="25">
         <v>43662.630076076384</v>
       </c>
@@ -15934,7 +15934,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="398" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A398" s="25">
         <v>43662.638398935189</v>
       </c>
@@ -15963,7 +15963,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="399" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A399" s="25">
         <v>43662.651400266201</v>
       </c>
@@ -15992,7 +15992,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="400" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="25">
         <v>43662.653115231486</v>
       </c>
@@ -16021,7 +16021,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="401" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A401" s="25">
         <v>43662.868660763888</v>
       </c>
@@ -16050,7 +16050,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="402" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A402" s="25">
         <v>43665.537839201388</v>
       </c>
@@ -16079,7 +16079,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="403" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A403" s="25">
         <v>43665.538775069443</v>
       </c>
@@ -16102,7 +16102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A404" s="25">
         <v>43665.565719756945</v>
       </c>
@@ -16131,7 +16131,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="405" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A405" s="25">
         <v>43665.602270196759</v>
       </c>
@@ -16996,7 +16996,7 @@
       <c r="Z423" s="36"/>
       <c r="AA423" s="36"/>
     </row>
-    <row r="424" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:27" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A424" s="35">
         <v>43677.509918981479</v>
       </c>
@@ -18970,7 +18970,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="469" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A469" s="50">
         <v>43691.5980102662</v>
       </c>
@@ -20000,7 +20000,7 @@
       <c r="O496" s="48"/>
       <c r="P496" s="47"/>
     </row>
-    <row r="497" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A497" s="50">
         <v>43692.463983391208</v>
       </c>
@@ -20292,7 +20292,7 @@
       <c r="O504" s="47"/>
       <c r="P504" s="47"/>
     </row>
-    <row r="505" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A505" s="50">
         <v>43699.54147059028</v>
       </c>
@@ -21304,7 +21304,7 @@
       <c r="O532" s="48"/>
       <c r="P532" s="47"/>
     </row>
-    <row r="533" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A533" s="50">
         <v>43706.430542476854</v>
       </c>
@@ -22086,7 +22086,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="554" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A554" s="50">
         <v>43712.399156678242</v>
       </c>
@@ -22124,7 +22124,7 @@
         <v>2565</v>
       </c>
     </row>
-    <row r="555" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A555" s="50">
         <v>43712.407757083332</v>
       </c>
@@ -22162,7 +22162,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="556" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A556" s="50">
         <v>43712.409943379629</v>
       </c>
@@ -22198,7 +22198,7 @@
       <c r="O556" s="48"/>
       <c r="P556" s="48"/>
     </row>
-    <row r="557" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="557" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A557" s="50">
         <v>43712.415547476849</v>
       </c>
@@ -22236,7 +22236,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="558" spans="1:16" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="558" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A558" s="50">
         <v>43712.421258125003</v>
       </c>
@@ -22274,7 +22274,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="559" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="559" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A559" s="50">
         <v>43712.424563483801</v>
       </c>
@@ -22312,7 +22312,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="560" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="560" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A560" s="50">
         <v>43712.432625416666</v>
       </c>
@@ -22350,7 +22350,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="561" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="561" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A561" s="50">
         <v>43712.440652013887</v>
       </c>
@@ -22388,7 +22388,7 @@
         <v>2981</v>
       </c>
     </row>
-    <row r="562" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="562" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A562" s="50">
         <v>43712.451808379628</v>
       </c>
@@ -22426,7 +22426,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="563" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="563" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A563" s="50">
         <v>43712.459328969911</v>
       </c>
@@ -22456,7 +22456,7 @@
       <c r="O563" s="47"/>
       <c r="P563" s="47"/>
     </row>
-    <row r="564" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="564" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A564" s="50">
         <v>43712.464040497682</v>
       </c>
@@ -22492,7 +22492,7 @@
       <c r="O564" s="48"/>
       <c r="P564" s="47"/>
     </row>
-    <row r="565" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="565" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A565" s="50">
         <v>43712.47561248843</v>
       </c>
@@ -22530,7 +22530,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="566" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="566" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A566" s="50">
         <v>43712.478235138886</v>
       </c>
@@ -22566,7 +22566,7 @@
       <c r="O566" s="48"/>
       <c r="P566" s="47"/>
     </row>
-    <row r="567" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="567" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A567" s="50">
         <v>43712.482904131946</v>
       </c>
@@ -22602,7 +22602,7 @@
       <c r="O567" s="48"/>
       <c r="P567" s="47"/>
     </row>
-    <row r="568" spans="1:16" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="568" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A568" s="50">
         <v>43712.486539513891</v>
       </c>
@@ -22640,7 +22640,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="569" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="569" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A569" s="50">
         <v>43712.486583101854</v>
       </c>
@@ -22672,7 +22672,7 @@
       <c r="O569" s="47"/>
       <c r="P569" s="47"/>
     </row>
-    <row r="570" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="570" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A570" s="50">
         <v>43712.518857824078</v>
       </c>
@@ -22710,7 +22710,7 @@
         <v>1917</v>
       </c>
     </row>
-    <row r="571" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="571" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A571" s="50">
         <v>43712.534898750004</v>
       </c>
@@ -22748,7 +22748,7 @@
         <v>3238</v>
       </c>
     </row>
-    <row r="572" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="572" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A572" s="50">
         <v>43712.535281874996</v>
       </c>
@@ -22780,7 +22780,7 @@
       <c r="O572" s="47"/>
       <c r="P572" s="47"/>
     </row>
-    <row r="573" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="573" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A573" s="50">
         <v>43712.545961504627</v>
       </c>
@@ -22818,7 +22818,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="574" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="574" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A574" s="50">
         <v>43712.554804884261</v>
       </c>
@@ -22856,7 +22856,7 @@
         <v>2214</v>
       </c>
     </row>
-    <row r="575" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="575" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A575" s="50">
         <v>43712.568402986115</v>
       </c>
@@ -22892,7 +22892,7 @@
       <c r="O575" s="48"/>
       <c r="P575" s="47"/>
     </row>
-    <row r="576" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="576" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A576" s="50">
         <v>43712.570633854164</v>
       </c>
@@ -22930,7 +22930,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="577" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="577" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A577" s="50">
         <v>43712.593498831018</v>
       </c>
@@ -22962,7 +22962,7 @@
       <c r="O577" s="47"/>
       <c r="P577" s="47"/>
     </row>
-    <row r="578" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A578" s="50">
         <v>43712.60098609954</v>
       </c>
@@ -22998,7 +22998,7 @@
       <c r="O578" s="48"/>
       <c r="P578" s="47"/>
     </row>
-    <row r="579" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="579" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A579" s="50">
         <v>43712.637202280093</v>
       </c>
@@ -23036,7 +23036,7 @@
       <c r="O579" s="48"/>
       <c r="P579" s="47"/>
     </row>
-    <row r="580" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A580" s="50">
         <v>43712.648180833334</v>
       </c>
@@ -23074,7 +23074,7 @@
       <c r="O580" s="48"/>
       <c r="P580" s="47"/>
     </row>
-    <row r="581" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A581" s="50">
         <v>43713.424205613424</v>
       </c>
@@ -23106,7 +23106,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="582" spans="1:16" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A582" s="50">
         <v>43713.425145335648</v>
       </c>
@@ -23138,7 +23138,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="583" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="583" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A583" s="50">
         <v>43713.435373171291</v>
       </c>
@@ -23174,7 +23174,7 @@
       <c r="O583" s="48"/>
       <c r="P583" s="47"/>
     </row>
-    <row r="584" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A584" s="50">
         <v>43713.4464271412</v>
       </c>
@@ -23210,7 +23210,7 @@
       <c r="O584" s="48"/>
       <c r="P584" s="47"/>
     </row>
-    <row r="585" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="585" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A585" s="50">
         <v>43713.450989293982</v>
       </c>
@@ -23248,7 +23248,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="586" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="586" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A586" s="50">
         <v>43713.464215254629</v>
       </c>
@@ -23284,7 +23284,7 @@
       <c r="O586" s="48"/>
       <c r="P586" s="47"/>
     </row>
-    <row r="587" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="587" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A587" s="50">
         <v>43713.481925486107</v>
       </c>
@@ -23322,7 +23322,7 @@
       <c r="O587" s="48"/>
       <c r="P587" s="47"/>
     </row>
-    <row r="588" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="588" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A588" s="50">
         <v>43713.543691203704</v>
       </c>
@@ -23360,7 +23360,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="589" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A589" s="50">
         <v>43713.556214594908</v>
       </c>
@@ -23398,7 +23398,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="590" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="590" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A590" s="50">
         <v>43713.55751481482</v>
       </c>
@@ -23436,7 +23436,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="591" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="591" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A591" s="50">
         <v>43713.59901273148</v>
       </c>
@@ -23474,7 +23474,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="592" spans="1:16" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="592" spans="1:16" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A592" s="50">
         <v>43713.602299502316</v>
       </c>
@@ -24561,7 +24561,7 @@
       <c r="T617" s="36"/>
       <c r="U617" s="36"/>
     </row>
-    <row r="618" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="618" spans="1:21" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A618" s="35">
         <v>43720.398113425923</v>
       </c>
@@ -25592,7 +25592,7 @@
       <c r="T642" s="36"/>
       <c r="U642" s="36"/>
     </row>
-    <row r="643" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="643" spans="1:21" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A643" s="35">
         <v>43724.414629629631</v>
       </c>
@@ -25676,7 +25676,7 @@
       <c r="T644" s="36"/>
       <c r="U644" s="36"/>
     </row>
-    <row r="645" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="645" spans="1:21" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A645" s="35">
         <v>43724.422766203701</v>
       </c>
@@ -26840,10 +26840,15 @@
       <c r="U673" s="36"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P673">
-    <filterColumn colId="1">
+  <autoFilter ref="A1:AA673">
+    <filterColumn colId="7">
       <filters>
-        <filter val="SDR-751"/>
+        <filter val="14.5"/>
+        <filter val="15"/>
+        <filter val="16.8"/>
+        <filter val="17.5"/>
+        <filter val="21.5"/>
+        <filter val="50"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>